<commit_message>
Uploaded some written notes + added silence to test continuum files
</commit_message>
<xml_diff>
--- a/R/Concatenate Lists.xlsx
+++ b/R/Concatenate Lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF64B3F-F15A-4EF9-B872-6071C6CB19C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F3E100-2C68-42BD-B71F-5858FC365829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
@@ -125,13 +125,13 @@
     <t>b</t>
   </si>
   <si>
-    <t>Participant instructed to do the task for</t>
-  </si>
-  <si>
     <t xml:space="preserve">Versions of  experiment </t>
   </si>
   <si>
     <t>What qualities are assigned to the two talkers in the critical trials</t>
+  </si>
+  <si>
+    <t>which Talker the participant is instructed to perform the task for</t>
   </si>
 </sst>
 </file>
@@ -366,32 +366,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -402,23 +384,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,13 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC81691-9F24-4C87-8366-AE2912EBB662}">
   <dimension ref="A1:AA718"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="78" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="67" workbookViewId="0">
+      <selection activeCell="AE50" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="2.6328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.6328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" style="4" customWidth="1"/>
     <col min="4" max="7" width="10.6328125" style="1" customWidth="1"/>
@@ -776,14 +776,14 @@
       <c r="Y1" s="5"/>
     </row>
     <row r="2" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="27"/>
       <c r="I2" s="20" t="s">
         <v>24</v>
@@ -793,61 +793,61 @@
         <v>19</v>
       </c>
       <c r="L2" s="27"/>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
     </row>
     <row r="3" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="35"/>
+      <c r="K3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="41" t="s">
-        <v>29</v>
-      </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="31" t="s">
         <v>21</v>
       </c>
       <c r="N3" s="8"/>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
       <c r="R3" s="14"/>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
       <c r="V3" s="14"/>
-      <c r="W3" s="30" t="s">
+      <c r="W3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="31"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="45"/>
     </row>
     <row r="4" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
@@ -855,30 +855,30 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="44"/>
+      <c r="I4" s="42"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="37"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
       <c r="R4" s="7"/>
-      <c r="S4" s="32" t="s">
+      <c r="S4" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
       <c r="V4" s="7"/>
-      <c r="W4" s="32" t="s">
+      <c r="W4" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
@@ -897,9 +897,9 @@
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="44"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="37"/>
+      <c r="K5" s="41"/>
       <c r="M5" s="13"/>
       <c r="O5" s="10" t="s">
         <v>18</v>
@@ -961,7 +961,7 @@
       <c r="B7" s="18">
         <v>1</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -980,8 +980,8 @@
       <c r="I7" s="15">
         <v>1</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34" t="s">
+      <c r="J7" s="29"/>
+      <c r="K7" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="5"/>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B8" s="27"/>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -1037,7 +1037,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
-      <c r="K8" s="34"/>
+      <c r="K8" s="30"/>
       <c r="L8" s="5"/>
       <c r="O8" s="2" t="s">
         <v>18</v>
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C9" s="34"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1076,7 +1076,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="38"/>
+      <c r="K9" s="32"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -1093,7 +1093,7 @@
       <c r="Y9" s="21"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C10" s="34"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1102,8 +1102,8 @@
       <c r="I10" s="15">
         <v>2</v>
       </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34" t="s">
+      <c r="J10" s="29"/>
+      <c r="K10" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="5"/>
@@ -1149,7 +1149,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="34"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="5"/>
       <c r="O11" s="2" t="s">
         <v>17</v>
@@ -1182,7 +1182,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="39"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
@@ -1190,7 +1190,7 @@
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
-      <c r="K12" s="39"/>
+      <c r="K12" s="33"/>
       <c r="L12" s="17"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
@@ -1212,7 +1212,7 @@
       <c r="B13" s="18">
         <v>2</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="21" t="s">
@@ -1231,8 +1231,8 @@
       <c r="I13" s="15">
         <v>3</v>
       </c>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34" t="s">
+      <c r="J13" s="29"/>
+      <c r="K13" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L13" s="5"/>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -1288,7 +1288,7 @@
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
-      <c r="K14" s="34"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="5"/>
       <c r="O14" s="2" t="s">
         <v>18</v>
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C15" s="34"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1327,7 +1327,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="38"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
@@ -1344,7 +1344,7 @@
       <c r="Y15" s="21"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C16" s="34"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1353,8 +1353,8 @@
       <c r="I16" s="15">
         <v>4</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34" t="s">
+      <c r="J16" s="29"/>
+      <c r="K16" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L16" s="5"/>
@@ -1391,7 +1391,7 @@
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C17" s="34"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1399,7 +1399,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="34"/>
+      <c r="K17" s="30"/>
       <c r="L17" s="5"/>
       <c r="O17" s="2" t="s">
         <v>17</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B18" s="18"/>
-      <c r="C18" s="39"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="23"/>
       <c r="E18" s="24"/>
       <c r="F18" s="16"/>
@@ -1459,7 +1459,7 @@
       <c r="B19" s="18">
         <v>3</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -1478,8 +1478,8 @@
       <c r="I19" s="15">
         <v>5</v>
       </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34" t="s">
+      <c r="J19" s="29"/>
+      <c r="K19" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L19" s="5"/>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="21" t="s">
@@ -1535,7 +1535,7 @@
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
       <c r="J20" s="26"/>
-      <c r="K20" s="34"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="5"/>
       <c r="O20" s="2" t="s">
         <v>18</v>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C21" s="34"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1574,7 +1574,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="38"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
@@ -1591,7 +1591,7 @@
       <c r="Y21" s="21"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C22" s="34"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1600,8 +1600,8 @@
       <c r="I22" s="15">
         <v>6</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="40" t="s">
+      <c r="J22" s="29"/>
+      <c r="K22" s="34" t="s">
         <v>5</v>
       </c>
       <c r="L22" s="26"/>
@@ -1638,7 +1638,7 @@
       </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C23" s="34"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1646,7 +1646,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="40"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="26"/>
       <c r="O23" s="2" t="s">
         <v>17</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B24" s="18"/>
-      <c r="C24" s="39"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="23"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -1686,7 +1686,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
-      <c r="K24" s="39"/>
+      <c r="K24" s="33"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -1706,7 +1706,7 @@
       <c r="B25" s="18">
         <v>4</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="21" t="s">
@@ -1725,8 +1725,8 @@
       <c r="I25" s="15">
         <v>7</v>
       </c>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34" t="s">
+      <c r="J25" s="29"/>
+      <c r="K25" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L25" s="5"/>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="21" t="s">
@@ -1782,7 +1782,7 @@
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="34"/>
+      <c r="K26" s="30"/>
       <c r="L26" s="5"/>
       <c r="O26" s="2" t="s">
         <v>18</v>
@@ -1813,7 +1813,7 @@
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C27" s="34"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1821,7 +1821,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
-      <c r="K27" s="38"/>
+      <c r="K27" s="32"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
@@ -1838,7 +1838,7 @@
       <c r="Y27" s="21"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C28" s="34"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1847,15 +1847,15 @@
       <c r="I28" s="15">
         <v>8</v>
       </c>
-      <c r="J28" s="33"/>
-      <c r="K28" s="34" t="s">
+      <c r="J28" s="29"/>
+      <c r="K28" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="15">
         <v>1</v>
       </c>
-      <c r="N28" s="33"/>
+      <c r="N28" s="29"/>
       <c r="O28" s="2" t="s">
         <v>18</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C29" s="34"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1895,7 +1895,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="34"/>
+      <c r="K29" s="30"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B30" s="18"/>
-      <c r="C30" s="39"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="23"/>
       <c r="E30" s="16"/>
       <c r="F30" s="17"/>
@@ -1959,7 +1959,7 @@
       <c r="B31" s="18">
         <v>5</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="21" t="s">
@@ -1978,8 +1978,8 @@
       <c r="I31" s="15">
         <v>9</v>
       </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="34" t="s">
+      <c r="J31" s="29"/>
+      <c r="K31" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L31" s="5"/>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="21" t="s">
@@ -2035,7 +2035,7 @@
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
-      <c r="K32" s="34"/>
+      <c r="K32" s="30"/>
       <c r="L32" s="5"/>
       <c r="O32" s="2" t="s">
         <v>18</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B33" s="9"/>
-      <c r="C33" s="34"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
@@ -2075,7 +2075,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
-      <c r="K33" s="38"/>
+      <c r="K33" s="32"/>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B34" s="9"/>
-      <c r="C34" s="34"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
@@ -2102,8 +2102,8 @@
       <c r="I34" s="15">
         <v>10</v>
       </c>
-      <c r="J34" s="33"/>
-      <c r="K34" s="34" t="s">
+      <c r="J34" s="29"/>
+      <c r="K34" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L34" s="5"/>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B35" s="9"/>
-      <c r="C35" s="34"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
@@ -2149,7 +2149,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="34"/>
+      <c r="K35" s="30"/>
       <c r="L35" s="5"/>
       <c r="O35" s="2" t="s">
         <v>17</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B36" s="15"/>
-      <c r="C36" s="39"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="23"/>
       <c r="E36" s="24"/>
       <c r="F36" s="23"/>
@@ -2189,7 +2189,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
-      <c r="K36" s="39"/>
+      <c r="K36" s="33"/>
       <c r="L36" s="17"/>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
@@ -2209,7 +2209,7 @@
       <c r="B37" s="18">
         <v>6</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="21" t="s">
@@ -2228,8 +2228,8 @@
       <c r="I37" s="15">
         <v>11</v>
       </c>
-      <c r="J37" s="33"/>
-      <c r="K37" s="34" t="s">
+      <c r="J37" s="29"/>
+      <c r="K37" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L37" s="5"/>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="21" t="s">
@@ -2285,7 +2285,7 @@
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
-      <c r="K38" s="34"/>
+      <c r="K38" s="30"/>
       <c r="L38" s="5"/>
       <c r="O38" s="2" t="s">
         <v>18</v>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C39" s="34"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="2"/>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
@@ -2324,7 +2324,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
-      <c r="K39" s="38"/>
+      <c r="K39" s="32"/>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
@@ -2341,7 +2341,7 @@
       <c r="Y39" s="21"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C40" s="34"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="2"/>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
@@ -2350,8 +2350,8 @@
       <c r="I40" s="15">
         <v>12</v>
       </c>
-      <c r="J40" s="33"/>
-      <c r="K40" s="34" t="s">
+      <c r="J40" s="29"/>
+      <c r="K40" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L40" s="5"/>
@@ -2388,7 +2388,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C41" s="34"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3"/>
       <c r="F41" s="2"/>
@@ -2396,7 +2396,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="34"/>
+      <c r="K41" s="30"/>
       <c r="L41" s="5"/>
       <c r="O41" s="2" t="s">
         <v>17</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B42" s="18"/>
-      <c r="C42" s="39"/>
+      <c r="C42" s="33"/>
       <c r="D42" s="23"/>
       <c r="E42" s="24"/>
       <c r="F42" s="16"/>
@@ -2456,7 +2456,7 @@
       <c r="B43" s="18">
         <v>7</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="21" t="s">
@@ -2475,8 +2475,8 @@
       <c r="I43" s="15">
         <v>13</v>
       </c>
-      <c r="J43" s="33"/>
-      <c r="K43" s="34" t="s">
+      <c r="J43" s="29"/>
+      <c r="K43" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L43" s="5"/>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B44" s="27"/>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="21" t="s">
@@ -2532,7 +2532,7 @@
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
-      <c r="K44" s="34"/>
+      <c r="K44" s="30"/>
       <c r="L44" s="5"/>
       <c r="O44" s="2" t="s">
         <v>18</v>
@@ -2565,7 +2565,7 @@
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="9"/>
-      <c r="C45" s="34"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="2"/>
       <c r="E45" s="3"/>
       <c r="F45" s="2"/>
@@ -2573,7 +2573,7 @@
       <c r="H45" s="5"/>
       <c r="I45" s="25"/>
       <c r="J45" s="25"/>
-      <c r="K45" s="38"/>
+      <c r="K45" s="32"/>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
       <c r="N45" s="25"/>
@@ -2592,7 +2592,7 @@
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="34"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="2"/>
       <c r="E46" s="3"/>
       <c r="F46" s="2"/>
@@ -2601,8 +2601,8 @@
       <c r="I46" s="15">
         <v>14</v>
       </c>
-      <c r="J46" s="33"/>
-      <c r="K46" s="40" t="s">
+      <c r="J46" s="29"/>
+      <c r="K46" s="34" t="s">
         <v>5</v>
       </c>
       <c r="L46" s="26"/>
@@ -2641,7 +2641,7 @@
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="34"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="2"/>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
@@ -2649,7 +2649,7 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="40"/>
+      <c r="K47" s="34"/>
       <c r="L47" s="26"/>
       <c r="O47" s="2" t="s">
         <v>17</v>
@@ -2682,7 +2682,7 @@
     <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="15"/>
-      <c r="C48" s="39"/>
+      <c r="C48" s="33"/>
       <c r="D48" s="23"/>
       <c r="E48" s="24"/>
       <c r="F48" s="23"/>
@@ -2690,7 +2690,7 @@
       <c r="H48" s="16"/>
       <c r="I48" s="16"/>
       <c r="J48" s="16"/>
-      <c r="K48" s="39"/>
+      <c r="K48" s="33"/>
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
@@ -2710,7 +2710,7 @@
       <c r="B49" s="18">
         <v>8</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="21" t="s">
@@ -2729,8 +2729,8 @@
       <c r="I49" s="15">
         <v>15</v>
       </c>
-      <c r="J49" s="33"/>
-      <c r="K49" s="34" t="s">
+      <c r="J49" s="29"/>
+      <c r="K49" s="30" t="s">
         <v>4</v>
       </c>
       <c r="L49" s="5"/>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B50" s="27"/>
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="21" t="s">
@@ -2786,7 +2786,7 @@
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
       <c r="J50" s="26"/>
-      <c r="K50" s="34"/>
+      <c r="K50" s="30"/>
       <c r="L50" s="5"/>
       <c r="O50" s="2" t="s">
         <v>18</v>
@@ -2817,7 +2817,7 @@
       </c>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C51" s="34"/>
+      <c r="C51" s="30"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
       <c r="F51" s="2"/>
@@ -2825,7 +2825,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="25"/>
       <c r="J51" s="25"/>
-      <c r="K51" s="38"/>
+      <c r="K51" s="32"/>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -2842,7 +2842,7 @@
       <c r="Y51" s="21"/>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C52" s="34"/>
+      <c r="C52" s="30"/>
       <c r="D52" s="2"/>
       <c r="E52" s="3"/>
       <c r="F52" s="2"/>
@@ -2851,15 +2851,15 @@
       <c r="I52" s="15">
         <v>16</v>
       </c>
-      <c r="J52" s="33"/>
-      <c r="K52" s="34" t="s">
+      <c r="J52" s="29"/>
+      <c r="K52" s="30" t="s">
         <v>5</v>
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="15">
         <v>1</v>
       </c>
-      <c r="N52" s="33"/>
+      <c r="N52" s="29"/>
       <c r="O52" s="2" t="s">
         <v>18</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C53" s="34"/>
+      <c r="C53" s="30"/>
       <c r="D53" s="2"/>
       <c r="E53" s="3"/>
       <c r="F53" s="2"/>
@@ -2934,14 +2934,30 @@
       </c>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="X54" s="1"/>
-      <c r="Y54" s="1"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17"/>
+      <c r="S54" s="17"/>
+      <c r="T54" s="17"/>
+      <c r="U54" s="17"/>
+      <c r="V54" s="17"/>
+      <c r="W54" s="17"/>
+      <c r="X54" s="17"/>
+      <c r="Y54" s="16"/>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>

</xml_diff>

<commit_message>
Test File Combinations & Naming
</commit_message>
<xml_diff>
--- a/R/Concatenate Lists.xlsx
+++ b/R/Concatenate Lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F3E100-2C68-42BD-B71F-5858FC365829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EAFD97-D995-4407-B763-619989E89571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="33">
   <si>
     <t>Critical Items</t>
   </si>
@@ -83,12 +83,6 @@
     <t>Set C</t>
   </si>
   <si>
-    <t>Ear Inversion</t>
-  </si>
-  <si>
-    <t>Gender Inversion</t>
-  </si>
-  <si>
     <t>Nonword</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
   </si>
   <si>
     <t>Attended Talker</t>
-  </si>
-  <si>
-    <t>Ear &amp; Gender Inversion</t>
   </si>
   <si>
     <t>Version</t>
@@ -132,6 +123,18 @@
   </si>
   <si>
     <t>which Talker the participant is instructed to perform the task for</t>
+  </si>
+  <si>
+    <t>2/4 lists the will be run initially</t>
+  </si>
+  <si>
+    <t>Attended Talker Nonword: Same Ear</t>
+  </si>
+  <si>
+    <t>Attended Talker Nonword: Opposite Ear</t>
+  </si>
+  <si>
+    <t>Attended Talker Word: Opposite Ear</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -276,11 +279,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,12 +333,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -387,6 +404,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,6 +441,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -734,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC81691-9F24-4C87-8366-AE2912EBB662}">
-  <dimension ref="A1:AA718"/>
+  <dimension ref="A1:AD718"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="67" workbookViewId="0">
-      <selection activeCell="AE50" sqref="AE50"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -761,11 +817,11 @@
     <col min="22" max="22" width="2.6328125" style="1" customWidth="1"/>
     <col min="23" max="23" width="10.6328125" style="1" customWidth="1"/>
     <col min="24" max="25" width="10.6328125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="2.6328125" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.7265625" style="1"/>
+    <col min="26" max="27" width="2.6328125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
@@ -775,7 +831,7 @@
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
@@ -784,15 +840,15 @@
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="27"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="25"/>
       <c r="M2" s="36" t="s">
         <v>11</v>
       </c>
@@ -809,26 +865,26 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
-      <c r="H3" s="35"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="J3" s="33"/>
       <c r="K3" s="40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="31" t="s">
-        <v>21</v>
+      <c r="M3" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="43" t="s">
@@ -836,20 +892,20 @@
       </c>
       <c r="P3" s="44"/>
       <c r="Q3" s="44"/>
-      <c r="R3" s="14"/>
+      <c r="R3" s="12"/>
       <c r="S3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
-      <c r="V3" s="14"/>
+      <c r="V3" s="12"/>
       <c r="W3" s="43" t="s">
         <v>14</v>
       </c>
       <c r="X3" s="43"/>
       <c r="Y3" s="45"/>
     </row>
-    <row r="4" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -860,29 +916,29 @@
       <c r="K4" s="41"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="O4" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
       <c r="R4" s="7"/>
       <c r="S4" s="46" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="T4" s="46"/>
       <c r="U4" s="46"/>
       <c r="V4" s="7"/>
       <c r="W4" s="46" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="X4" s="46"/>
       <c r="Y4" s="46"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -900,246 +956,268 @@
       <c r="I5" s="42"/>
       <c r="J5" s="4"/>
       <c r="K5" s="41"/>
-      <c r="M5" s="13"/>
+      <c r="M5" s="11"/>
       <c r="O5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="P5" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="35" t="s">
         <v>3</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="T5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="T5" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="35" t="s">
         <v>3</v>
       </c>
       <c r="V5" s="4"/>
       <c r="W5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="X5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="X5" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B7" s="18">
+    <row r="6" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="16"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="14"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="47"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="22" t="s">
+      <c r="D7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="15">
+      <c r="H7" s="24"/>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30" t="s">
+      <c r="J7" s="27"/>
+      <c r="K7" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="5"/>
-      <c r="M7" s="18">
+      <c r="M7" s="16">
         <v>1</v>
       </c>
-      <c r="N7" s="27"/>
+      <c r="N7" s="25"/>
       <c r="O7" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B8" s="27"/>
-      <c r="C8" s="32" t="s">
+      <c r="AA7" s="51"/>
+      <c r="AB7" s="48"/>
+      <c r="AC7" s="49"/>
+      <c r="AD7" s="47"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B8" s="25"/>
+      <c r="C8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="22" t="s">
+      <c r="D8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="30"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="28"/>
       <c r="L8" s="5"/>
       <c r="O8" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C9" s="30"/>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="48"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="47"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C9" s="28"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
       <c r="O9" s="19"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="19"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="17"/>
       <c r="S9" s="19"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="19"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="17"/>
       <c r="W9" s="19"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C10" s="30"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="19"/>
+      <c r="AA9" s="51"/>
+      <c r="AB9" s="48"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="47"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C10" s="28"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <v>2</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30" t="s">
+      <c r="J10" s="27"/>
+      <c r="K10" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="16">
         <v>2</v>
       </c>
-      <c r="N10" s="27"/>
+      <c r="N10" s="25"/>
       <c r="O10" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AA10" s="51"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="47"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1149,249 +1227,253 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="30"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="5"/>
       <c r="O11" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="48"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="47"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B13" s="18">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B13" s="16">
         <v>2</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="D13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="15">
+      <c r="H13" s="24"/>
+      <c r="I13" s="13">
         <v>3</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="30" t="s">
+      <c r="J13" s="27"/>
+      <c r="K13" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="16">
         <v>3</v>
       </c>
-      <c r="N13" s="27"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B14" s="27"/>
-      <c r="C14" s="32" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B14" s="25"/>
+      <c r="C14" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="22" t="s">
+      <c r="D14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="30"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="28"/>
       <c r="L14" s="5"/>
       <c r="O14" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C15" s="30"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C15" s="28"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
       <c r="O15" s="19"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="19"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="19"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="19"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="17"/>
       <c r="W15" s="19"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C16" s="30"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="19"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C16" s="28"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="15">
+      <c r="I16" s="13">
         <v>4</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30" t="s">
+      <c r="J16" s="27"/>
+      <c r="K16" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L16" s="5"/>
-      <c r="M16" s="18">
+      <c r="M16" s="16">
         <v>4</v>
       </c>
-      <c r="N16" s="27"/>
+      <c r="N16" s="25"/>
       <c r="O16" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C17" s="30"/>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C17" s="28"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1399,246 +1481,263 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="30"/>
+      <c r="K17" s="28"/>
       <c r="L17" s="5"/>
       <c r="O17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B18" s="18"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B19" s="18">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B18" s="16"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC18" s="55"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B19" s="16">
         <v>3</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="22" t="s">
+      <c r="D19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="15">
+      <c r="H19" s="24"/>
+      <c r="I19" s="13">
         <v>5</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30" t="s">
+      <c r="J19" s="27"/>
+      <c r="K19" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L19" s="5"/>
-      <c r="M19" s="20">
+      <c r="M19" s="18">
         <v>4</v>
       </c>
-      <c r="N19" s="27"/>
+      <c r="N19" s="25"/>
       <c r="O19" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y19" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B20" s="27"/>
-      <c r="C20" s="32" t="s">
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="48"/>
+      <c r="AC19" s="55"/>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B20" s="25"/>
+      <c r="C20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="22" t="s">
+      <c r="D20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="30"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="28"/>
       <c r="L20" s="5"/>
       <c r="O20" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y20" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C21" s="30"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="55"/>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C21" s="28"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="19"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="25"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="23"/>
       <c r="S21" s="19"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="25"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="23"/>
       <c r="W21" s="19"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C22" s="30"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="19"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="55"/>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C22" s="28"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="15">
+      <c r="I22" s="13">
         <v>6</v>
       </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="34" t="s">
+      <c r="J22" s="27"/>
+      <c r="K22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="20">
+      <c r="L22" s="24"/>
+      <c r="M22" s="18">
         <v>3</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="25"/>
       <c r="O22" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y22" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C23" s="30"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="55"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C23" s="28"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1646,248 +1745,251 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="26"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="24"/>
       <c r="O23" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B24" s="18"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="16"/>
-    </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B25" s="18">
+      <c r="AA23" s="53"/>
+      <c r="AB23" s="48"/>
+      <c r="AC23" s="55"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B24" s="16"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B25" s="16">
         <v>4</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="22" t="s">
+      <c r="D25" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="15">
+      <c r="H25" s="24"/>
+      <c r="I25" s="13">
         <v>7</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="30" t="s">
+      <c r="J25" s="27"/>
+      <c r="K25" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L25" s="5"/>
-      <c r="M25" s="20">
+      <c r="M25" s="18">
         <v>2</v>
       </c>
-      <c r="N25" s="27"/>
+      <c r="N25" s="25"/>
       <c r="O25" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B26" s="27"/>
-      <c r="C26" s="32" t="s">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B26" s="25"/>
+      <c r="C26" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="22" t="s">
+      <c r="D26" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="30"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="28"/>
       <c r="L26" s="5"/>
       <c r="O26" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C27" s="30"/>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C27" s="28"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
       <c r="O27" s="19"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="19"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="17"/>
       <c r="S27" s="19"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-      <c r="V27" s="19"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="17"/>
       <c r="W27" s="19"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21"/>
-    </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C28" s="30"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="19"/>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C28" s="28"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="15">
+      <c r="I28" s="13">
         <v>8</v>
       </c>
-      <c r="J28" s="29"/>
-      <c r="K28" s="30" t="s">
+      <c r="J28" s="27"/>
+      <c r="K28" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L28" s="5"/>
-      <c r="M28" s="15">
+      <c r="M28" s="13">
         <v>1</v>
       </c>
-      <c r="N28" s="29"/>
+      <c r="N28" s="27"/>
       <c r="O28" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R28" s="5"/>
       <c r="S28" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V28" s="5"/>
       <c r="W28" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C29" s="30"/>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="C29" s="28"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1895,171 +1997,171 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="30"/>
+      <c r="K29" s="28"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="R29" s="5"/>
       <c r="S29" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="V29" s="5"/>
       <c r="W29" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B30" s="18"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="16"/>
-    </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B31" s="18">
+    <row r="30" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B30" s="16"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="14"/>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B31" s="16">
         <v>5</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="22" t="s">
+      <c r="D31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="15">
+      <c r="H31" s="24"/>
+      <c r="I31" s="13">
         <v>9</v>
       </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="30" t="s">
+      <c r="J31" s="27"/>
+      <c r="K31" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L31" s="5"/>
-      <c r="M31" s="20">
+      <c r="M31" s="18">
         <v>1</v>
       </c>
-      <c r="N31" s="27"/>
+      <c r="N31" s="25"/>
       <c r="O31" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B32" s="27"/>
-      <c r="C32" s="32" t="s">
+    <row r="32" spans="2:29" x14ac:dyDescent="0.35">
+      <c r="B32" s="25"/>
+      <c r="C32" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="21" t="s">
+      <c r="D32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="30"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="5"/>
       <c r="O32" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y32" s="2" t="s">
         <v>8</v>
@@ -2067,73 +2169,73 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B33" s="9"/>
-      <c r="C33" s="30"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
       <c r="G33" s="3"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="19"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="17"/>
       <c r="S33" s="19"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="19"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="17"/>
       <c r="W33" s="19"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="19"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B34" s="9"/>
-      <c r="C34" s="30"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
       <c r="G34" s="3"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="15">
+      <c r="I34" s="13">
         <v>10</v>
       </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="30" t="s">
+      <c r="J34" s="27"/>
+      <c r="K34" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L34" s="5"/>
-      <c r="M34" s="20">
+      <c r="M34" s="18">
         <v>2</v>
       </c>
-      <c r="N34" s="27"/>
+      <c r="N34" s="25"/>
       <c r="O34" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y34" s="2" t="s">
         <v>9</v>
@@ -2141,7 +2243,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B35" s="9"/>
-      <c r="C35" s="30"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
@@ -2149,246 +2251,246 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="30"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="5"/>
       <c r="O35" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B36" s="13"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B37" s="16">
         <v>6</v>
       </c>
-      <c r="Y35" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B36" s="15"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="28"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="16"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B37" s="18">
+      <c r="C37" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="G37" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="I37" s="13">
+        <v>11</v>
+      </c>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="21" t="s">
+      <c r="L37" s="5"/>
+      <c r="M37" s="18">
+        <v>3</v>
+      </c>
+      <c r="N37" s="25"/>
+      <c r="O37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="15">
-        <v>11</v>
-      </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="L37" s="5"/>
-      <c r="M37" s="20">
-        <v>3</v>
-      </c>
-      <c r="N37" s="27"/>
-      <c r="O37" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="P37" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y37" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B38" s="27"/>
-      <c r="C38" s="32" t="s">
+      <c r="B38" s="25"/>
+      <c r="C38" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="21" t="s">
+      <c r="D38" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="30"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="28"/>
       <c r="L38" s="5"/>
       <c r="O38" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y38" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C39" s="30"/>
+      <c r="C39" s="28"/>
       <c r="D39" s="2"/>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
       <c r="G39" s="3"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
       <c r="O39" s="19"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="19"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="17"/>
       <c r="S39" s="19"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="19"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="17"/>
       <c r="W39" s="19"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="19"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C40" s="30"/>
+      <c r="C40" s="28"/>
       <c r="D40" s="2"/>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
       <c r="G40" s="3"/>
       <c r="H40" s="5"/>
-      <c r="I40" s="15">
+      <c r="I40" s="13">
         <v>12</v>
       </c>
-      <c r="J40" s="29"/>
-      <c r="K40" s="30" t="s">
+      <c r="J40" s="27"/>
+      <c r="K40" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L40" s="5"/>
-      <c r="M40" s="20">
+      <c r="M40" s="18">
         <v>4</v>
       </c>
-      <c r="N40" s="27"/>
+      <c r="N40" s="25"/>
       <c r="O40" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U40" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y40" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C41" s="30"/>
+      <c r="C41" s="28"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3"/>
       <c r="F41" s="2"/>
@@ -2396,167 +2498,167 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="30"/>
+      <c r="K41" s="28"/>
       <c r="L41" s="5"/>
       <c r="O41" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y41" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B42" s="18"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="W42" s="16"/>
-      <c r="X42" s="16"/>
-      <c r="Y42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B43" s="18">
+      <c r="B43" s="16">
         <v>7</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F43" s="21" t="s">
+      <c r="D43" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="G43" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="26"/>
-      <c r="I43" s="15">
+      <c r="H43" s="24"/>
+      <c r="I43" s="13">
         <v>13</v>
       </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="30" t="s">
+      <c r="J43" s="27"/>
+      <c r="K43" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L43" s="5"/>
-      <c r="M43" s="20">
+      <c r="M43" s="18">
         <v>4</v>
       </c>
-      <c r="N43" s="27"/>
+      <c r="N43" s="25"/>
       <c r="O43" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B44" s="27"/>
-      <c r="C44" s="32" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="21" t="s">
+      <c r="D44" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="30"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="28"/>
       <c r="L44" s="5"/>
       <c r="O44" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y44" s="2" t="s">
         <v>8</v>
@@ -2565,74 +2667,74 @@
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="9"/>
-      <c r="C45" s="30"/>
+      <c r="C45" s="28"/>
       <c r="D45" s="2"/>
       <c r="E45" s="3"/>
       <c r="F45" s="2"/>
       <c r="G45" s="3"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
       <c r="O45" s="19"/>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="21"/>
-      <c r="R45" s="25"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="23"/>
       <c r="S45" s="19"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="25"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="23"/>
       <c r="W45" s="19"/>
-      <c r="X45" s="21"/>
-      <c r="Y45" s="21"/>
+      <c r="X45" s="17"/>
+      <c r="Y45" s="19"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="30"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="2"/>
       <c r="E46" s="3"/>
       <c r="F46" s="2"/>
       <c r="G46" s="3"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="15">
+      <c r="I46" s="13">
         <v>14</v>
       </c>
-      <c r="J46" s="29"/>
-      <c r="K46" s="34" t="s">
+      <c r="J46" s="27"/>
+      <c r="K46" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L46" s="26"/>
-      <c r="M46" s="20">
+      <c r="L46" s="24"/>
+      <c r="M46" s="18">
         <v>3</v>
       </c>
-      <c r="N46" s="27"/>
+      <c r="N46" s="25"/>
       <c r="O46" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X46" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y46" s="2" t="s">
         <v>9</v>
@@ -2641,7 +2743,7 @@
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="30"/>
+      <c r="C47" s="28"/>
       <c r="D47" s="2"/>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
@@ -2649,31 +2751,31 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="26"/>
+      <c r="K47" s="32"/>
+      <c r="L47" s="24"/>
       <c r="O47" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X47" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y47" s="2" t="s">
         <v>8</v>
@@ -2681,217 +2783,217 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="23"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
-      <c r="S48" s="16"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="16"/>
-      <c r="V48" s="16"/>
-      <c r="W48" s="16"/>
-      <c r="X48" s="23"/>
-      <c r="Y48" s="16"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="21"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B49" s="18">
+      <c r="B49" s="16">
         <v>8</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" s="21" t="s">
+      <c r="D49" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="26"/>
-      <c r="I49" s="15">
+      <c r="H49" s="24"/>
+      <c r="I49" s="13">
         <v>15</v>
       </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="30" t="s">
+      <c r="J49" s="27"/>
+      <c r="K49" s="28" t="s">
         <v>4</v>
       </c>
       <c r="L49" s="5"/>
-      <c r="M49" s="20">
+      <c r="M49" s="18">
         <v>2</v>
       </c>
-      <c r="N49" s="27"/>
+      <c r="N49" s="25"/>
       <c r="O49" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U49" s="2" t="s">
         <v>9</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y49" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B50" s="27"/>
-      <c r="C50" s="32" t="s">
+      <c r="B50" s="25"/>
+      <c r="C50" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="21" t="s">
+      <c r="D50" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="30"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="28"/>
       <c r="L50" s="5"/>
       <c r="O50" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X50" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y50" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C51" s="30"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
       <c r="F51" s="2"/>
       <c r="G51" s="3"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
       <c r="O51" s="19"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="19"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="17"/>
       <c r="S51" s="19"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="19"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="19"/>
+      <c r="V51" s="17"/>
       <c r="W51" s="19"/>
-      <c r="X51" s="21"/>
-      <c r="Y51" s="21"/>
+      <c r="X51" s="17"/>
+      <c r="Y51" s="19"/>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C52" s="30"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="2"/>
       <c r="E52" s="3"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3"/>
       <c r="H52" s="5"/>
-      <c r="I52" s="15">
+      <c r="I52" s="13">
         <v>16</v>
       </c>
-      <c r="J52" s="29"/>
-      <c r="K52" s="30" t="s">
+      <c r="J52" s="27"/>
+      <c r="K52" s="28" t="s">
         <v>5</v>
       </c>
       <c r="L52" s="5"/>
-      <c r="M52" s="15">
+      <c r="M52" s="13">
         <v>1</v>
       </c>
-      <c r="N52" s="29"/>
+      <c r="N52" s="27"/>
       <c r="O52" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R52" s="5"/>
       <c r="S52" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V52" s="5"/>
       <c r="W52" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X52" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Y52" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="C53" s="30"/>
+      <c r="C53" s="28"/>
       <c r="D53" s="2"/>
       <c r="E53" s="3"/>
       <c r="F53" s="2"/>
@@ -2904,60 +3006,60 @@
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
       <c r="O53" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="R53" s="5"/>
       <c r="S53" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="U53" s="2" t="s">
         <v>8</v>
       </c>
       <c r="V53" s="5"/>
       <c r="W53" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="X53" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Y53" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-      <c r="Q54" s="17"/>
-      <c r="R54" s="17"/>
-      <c r="S54" s="17"/>
-      <c r="T54" s="17"/>
-      <c r="U54" s="17"/>
-      <c r="V54" s="17"/>
-      <c r="W54" s="17"/>
-      <c r="X54" s="17"/>
-      <c r="Y54" s="16"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
@@ -17950,7 +18052,9 @@
       <c r="Y718" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="AB6:AC11"/>
+    <mergeCell ref="AB18:AC23"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="M2:Y2"/>

</xml_diff>